<commit_message>
sort the data right before tracking, and update some necessary info like validity, crm
</commit_message>
<xml_diff>
--- a/untuk_cs/data_blast/rekap_himpunan/new/REKAP HIMPUNAN NOVEMBER 1097.xlsx
+++ b/untuk_cs/data_blast/rekap_himpunan/new/REKAP HIMPUNAN NOVEMBER 1097.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\isra holding company\untuk_cs\data_blast\rekap_himpunan\new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A7D487-A43B-4FCA-AD95-F85142994A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED3AF09-B75A-4A37-95D4-A7242ACCFC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{E6A3E62E-5D66-4B50-9BD7-84073BFF055E}"/>
   </bookViews>
@@ -19,22 +19,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -371,6 +362,24 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -453,24 +462,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -951,7 +942,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68DDD9AA-18E4-41B7-A1FD-A507842B6312}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{68DDD9AA-18E4-41B7-A1FD-A507842B6312}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G19" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0"/>
@@ -1066,7 +1057,7 @@
     <dataField name="Count of No" fld="0" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1078,7 +1069,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea field="6" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1087,7 +1078,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1102,7 +1093,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea field="6" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1135,11 +1126,11 @@
     <tableColumn id="2" xr3:uid="{846F95A7-4AFF-4AA2-8610-5ABB4EE014A9}" name="Donatur" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{24ED3E4E-D426-44C9-8BFD-9D89B593EE15}" name="Whatsapp" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{D68749F9-0350-4F3D-8DC5-5E08EFE8BCD1}" name="Payment Account" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{E7E853D8-6673-46D1-B91A-4EB3866F36D6}" name="Date Blast" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{9533C8DD-7BCF-4014-936E-950B5E1629E0}" name="Date" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{26C86FFE-5387-4F22-B253-833C653F6AD2}" name="Nomor CS" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{2BFE59B0-9C7E-4782-BBB4-0301FFF28F23}" name="Total" dataDxfId="6" dataCellStyle="Currency [0]"/>
-    <tableColumn id="10" xr3:uid="{689D86FB-765E-450F-BE01-75A89D61FA30}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{E7E853D8-6673-46D1-B91A-4EB3866F36D6}" name="Date Blast" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{9533C8DD-7BCF-4014-936E-950B5E1629E0}" name="Date" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{26C86FFE-5387-4F22-B253-833C653F6AD2}" name="Nomor CS" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{2BFE59B0-9C7E-4782-BBB4-0301FFF28F23}" name="Total" dataDxfId="7" dataCellStyle="Currency [0]"/>
+    <tableColumn id="10" xr3:uid="{689D86FB-765E-450F-BE01-75A89D61FA30}" name="Column1" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1410,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38323B66-263B-4886-B622-1C4E58ABF8A4}">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H30"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,10 +1491,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="7">
-        <v>45668</v>
+        <v>45962</v>
       </c>
       <c r="F3" s="7">
-        <v>45668</v>
+        <v>45962</v>
       </c>
       <c r="G3" s="8">
         <v>6285119990038</v>
@@ -2341,7 +2332,7 @@
     <mergeCell ref="R3:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G30" xr:uid="{3DA28642-D810-41A8-9368-250FE38EFB42}">

</xml_diff>